<commit_message>
add label project académie
</commit_message>
<xml_diff>
--- a/data/translations.wikidata.xlsx
+++ b/data/translations.wikidata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t xml:space="preserve">Correspondence between Henri Fantin-Latour and Otto Scholderer, 1858-1902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kunstsammlung der Académie Royale de Peinture et de Sculpture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La collection d'art de l’Académie royale de peinture et de sculpture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The art collection of the Académie Royale de Peinture et de Sculpture</t>
   </si>
   <si>
     <t xml:space="preserve">help_intro</t>
@@ -398,13 +410,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="30.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="1" style="1" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="11.57"/>
@@ -634,7 +646,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
@@ -648,7 +660,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="191.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -662,7 +674,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="191.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>68</v>
       </c>
@@ -676,7 +688,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -690,7 +702,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
@@ -704,7 +716,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
@@ -718,9 +730,23 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>84</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds missing DFK ids to data entries
</commit_message>
<xml_diff>
--- a/data/translations.wikidata.xlsx
+++ b/data/translations.wikidata.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="translations" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="translations" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">OwnReality. To Each His Own Reality</t>
   </si>
   <si>
+    <t xml:space="preserve">filter_or</t>
+  </si>
+  <si>
     <t xml:space="preserve">pb</t>
   </si>
   <si>
@@ -94,6 +97,9 @@
     <t xml:space="preserve">Palais Beauharnais – full inventory of the furniture, bronzes, paintings and other objects</t>
   </si>
   <si>
+    <t xml:space="preserve">filter_pb</t>
+  </si>
+  <si>
     <t xml:space="preserve">dfkv</t>
   </si>
   <si>
@@ -106,6 +112,15 @@
     <t xml:space="preserve">german and french reception of art between 1870 and 1960</t>
   </si>
   <si>
+    <t xml:space="preserve">filter_dfkv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deutsch-französische Kunstvermittlung von 1870-1961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">german and french reception of art between 1870 and 1961</t>
+  </si>
+  <si>
     <t xml:space="preserve">babue</t>
   </si>
   <si>
@@ -118,12 +133,18 @@
     <t xml:space="preserve">Picture archive Hans-Peter Bühler on 19th and 20th century painting</t>
   </si>
   <si>
+    <t xml:space="preserve">filter_babue</t>
+  </si>
+  <si>
     <t xml:space="preserve">wikidata</t>
   </si>
   <si>
     <t xml:space="preserve">Wikidata</t>
   </si>
   <si>
+    <t xml:space="preserve">filter_wikidata</t>
+  </si>
+  <si>
     <t xml:space="preserve">results</t>
   </si>
   <si>
@@ -193,6 +214,9 @@
     <t xml:space="preserve">Architrave – arts and architecture in Paris and Versailles in accounts by Baroque-Era German travellers</t>
   </si>
   <si>
+    <t xml:space="preserve">filter_av</t>
+  </si>
+  <si>
     <t xml:space="preserve">fs</t>
   </si>
   <si>
@@ -202,6 +226,15 @@
     <t xml:space="preserve">Correspondence between Henri Fantin-Latour and Otto Scholderer, 1858-1902</t>
   </si>
   <si>
+    <t xml:space="preserve">filter_fs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Briefwechsel zwischen Henri Fantin-Latour und Otto Scholderer, 1858–1903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correspondence between Henri Fantin-Latour and Otto Scholderer, 1858-1903</t>
+  </si>
+  <si>
     <t xml:space="preserve">ar</t>
   </si>
   <si>
@@ -212,6 +245,9 @@
   </si>
   <si>
     <t xml:space="preserve">The art collection of the Académie Royale de Peinture et de Sculpture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_ar</t>
   </si>
   <si>
     <t xml:space="preserve">help_intro</t>
@@ -405,15 +441,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -478,7 +620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -492,261 +634,373 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="1" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="191.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="1" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+    <row r="27" customFormat="false" ht="191.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+    <row r="28" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+    <row r="29" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>88</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>